<commit_message>
Actualizacion de bitacora de respaldos
</commit_message>
<xml_diff>
--- a/Respaldo/Bitacora de respaldos.xlsx
+++ b/Respaldo/Bitacora de respaldos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\Respaldo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\qtp\Respaldo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="8">
   <si>
     <t xml:space="preserve">Fecha </t>
   </si>
@@ -148,6 +148,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -156,9 +159,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G16"/>
+  <dimension ref="B1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="B14:G16"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,31 +455,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="8" t="s">
         <v>2</v>
       </c>
@@ -528,10 +528,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="10">
+      <c r="E6" s="11">
         <v>42097</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
@@ -545,11 +545,11 @@
         <v>4</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="10">
+      <c r="E7" s="11">
         <f t="shared" ref="E7" si="0">SUM(E6,7)</f>
         <v>42104</v>
       </c>
-      <c r="F7" s="11"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="1" t="s">
         <v>5</v>
       </c>
@@ -563,11 +563,11 @@
         <v>4</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="10">
+      <c r="E8" s="11">
         <f t="shared" ref="E8" si="2">SUM(E7+7)</f>
         <v>42111</v>
       </c>
-      <c r="F8" s="11"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="1" t="s">
         <v>5</v>
       </c>
@@ -706,25 +706,26 @@
         <v>7</v>
       </c>
     </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>42174</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8">
+        <v>42174</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
+  <mergeCells count="31">
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
@@ -737,6 +738,23 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>